<commit_message>
segundo parte 20 de abril de 2025
</commit_message>
<xml_diff>
--- a/ballon/resultados/suj1_2025-04-20.xlsx
+++ b/ballon/resultados/suj1_2025-04-20.xlsx
@@ -28,7 +28,7 @@
     <t>precisao</t>
   </si>
   <si>
-    <t>62.5%</t>
+    <t>76.5%</t>
   </si>
 </sst>
 </file>
@@ -408,13 +408,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
terceira parte 20 de abril de 2025
</commit_message>
<xml_diff>
--- a/ballon/resultados/suj1_2025-04-20.xlsx
+++ b/ballon/resultados/suj1_2025-04-20.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Pontos</t>
   </si>
   <si>
     <t>n_balaos</t>
-  </si>
-  <si>
-    <t>acertos_pedra</t>
   </si>
   <si>
     <t>precisao</t>
@@ -386,13 +383,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,22 +399,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>13</v>
       </c>
       <c r="B2">
         <v>17</v>
       </c>
-      <c r="C2">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>